<commit_message>
end of day Thursday 8.19
</commit_message>
<xml_diff>
--- a/Data/Meta_descriptions.xlsx
+++ b/Data/Meta_descriptions.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrickatwater/Documents/NSS/Capstone/Spotify_Playlist_Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrickatwater/Documents/NSS/Capstone/Spotify_Playlist_Project/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD3D742-41C6-9B45-B988-2E44ED541D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50DD4B1F-4A64-BD42-A15C-4817C46FBE20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" activeTab="1" xr2:uid="{6D5C5EE3-D0D4-3B42-97FB-0465CE85313E}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="28">
   <si>
     <t>acousticness</t>
   </si>
@@ -574,10 +574,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B31F4DE-8CCF-C640-8661-C64D840B8CB5}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A10" sqref="A10:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -657,51 +657,43 @@
         <v>25</v>
       </c>
     </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" t="s">
-        <v>26</v>
+      <c r="A13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="1" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>